<commit_message>
Document sprint 4 #44
</commit_message>
<xml_diff>
--- a/docs/md/anexos/Registro-tiempo.xlsx
+++ b/docs/md/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -270,9 +273,6 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,9 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,11 +329,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="70">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -500,146 +503,146 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -661,146 +664,146 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -822,146 +825,307 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -995,7 +1159,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="55" headerRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="69" headerRowBorderDxfId="68">
   <autoFilter ref="B17:G26">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1005,19 +1169,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="52" totalsRowDxfId="53"/>
-    <tableColumn id="2" name="Min." dataDxfId="50" totalsRowDxfId="51"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="48" totalsRowDxfId="49"/>
-    <tableColumn id="4" name="Total" dataDxfId="46" totalsRowDxfId="47"/>
-    <tableColumn id="5" name="Real" dataDxfId="44" totalsRowDxfId="45"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43"/>
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="41" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="55" headerRowBorderDxfId="54">
   <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1027,19 +1191,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="38" totalsRowDxfId="39"/>
-    <tableColumn id="2" name="Min." dataDxfId="36" totalsRowDxfId="37"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="34" totalsRowDxfId="35"/>
-    <tableColumn id="4" name="Total" dataDxfId="32" totalsRowDxfId="33"/>
-    <tableColumn id="5" name="Real" dataDxfId="30" totalsRowDxfId="31"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="29"/>
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="27" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="41" headerRowBorderDxfId="40">
   <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1049,19 +1213,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="25"/>
-    <tableColumn id="2" name="Min." dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="4" name="Total" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="5" name="Real" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="13" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="27" headerRowBorderDxfId="26">
   <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1070,6 +1234,21 @@
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
     <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
@@ -1345,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G54"/>
+  <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,959 +1538,1195 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>15</v>
       </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
         <f>D4*C4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="18">
         <f>F4*C4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>45</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>8</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <f t="shared" ref="E5:E11" si="0">D5*C5</f>
         <v>360</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>7</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="19">
         <f t="shared" ref="G5:G11" si="1">F5*C5</f>
         <v>315</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>120</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>2</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>300</v>
       </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="14">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21">
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
+      <c r="B8" s="15">
         <v>8</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>720</v>
       </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="14">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="B9" s="15">
         <v>13</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>1440</v>
       </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="14">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21">
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
+      <c r="B10" s="15">
         <v>21</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <f>2.5*24*60</f>
         <v>3600</v>
       </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="14">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21">
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17">
+      <c r="B11" s="15">
         <v>40</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <f>7*24*60</f>
         <v>10080</v>
       </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="22">
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="7" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f>SUM(E4:E11)/60</f>
         <v>8</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="17">
         <f>SUM(G4:G11)/60</f>
         <v>9.25</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+      <c r="B18" s="14">
         <v>1</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>15</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <f>D18*C18</f>
         <v>15</v>
       </c>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="20">
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
         <f>F18*C18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="17">
+      <c r="B19" s="15">
         <v>2</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="10">
         <v>45</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="10">
         <f t="shared" ref="E19:E25" si="2">D19*C19</f>
         <v>180</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="12">
         <v>3</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="19">
         <f t="shared" ref="G19:G25" si="3">F19*C19</f>
         <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="17">
+      <c r="B20" s="15">
         <v>3</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="10">
         <v>120</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>2</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="10">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="12">
         <v>3</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="19">
         <f t="shared" si="3"/>
         <v>360</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="17">
+      <c r="B21" s="15">
         <v>5</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="10">
         <v>300</v>
       </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="12">
         <v>1</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="19">
         <f t="shared" si="3"/>
         <v>300</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="17">
+      <c r="B22" s="15">
         <v>8</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <v>720</v>
       </c>
-      <c r="D22" s="11">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" s="14">
-        <v>0</v>
-      </c>
-      <c r="G22" s="21">
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="17">
+      <c r="B23" s="15">
         <v>13</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="10">
         <v>1440</v>
       </c>
-      <c r="D23" s="11">
-        <v>0</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="14">
-        <v>0</v>
-      </c>
-      <c r="G23" s="21">
+      <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="17">
+      <c r="B24" s="15">
         <v>21</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="10">
         <f>2.5*24*60</f>
         <v>3600</v>
       </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="14">
-        <v>0</v>
-      </c>
-      <c r="G24" s="21">
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17">
+      <c r="B25" s="15">
         <v>40</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="10">
         <f>7*24*60</f>
         <v>10080</v>
       </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="14">
-        <v>0</v>
-      </c>
-      <c r="G25" s="22">
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="7" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f>SUM(E18:E25)/60</f>
         <v>7.25</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="17">
         <f>SUM(G18:G25)/60</f>
         <v>13.25</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="16">
+      <c r="B32" s="14">
         <v>1</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="8">
         <v>15</v>
       </c>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="D32" s="7">
+        <v>0</v>
+      </c>
+      <c r="E32" s="8">
         <f>D32*C32</f>
         <v>0</v>
       </c>
-      <c r="F32" s="13">
-        <v>0</v>
-      </c>
-      <c r="G32" s="20">
+      <c r="F32" s="11">
+        <v>0</v>
+      </c>
+      <c r="G32" s="18">
         <f>F32*C32</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="17">
+      <c r="B33" s="15">
         <v>2</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="10">
         <v>45</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>1</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="10">
         <f t="shared" ref="E33:E39" si="4">D33*C33</f>
         <v>45</v>
       </c>
-      <c r="F33" s="14">
-        <v>0</v>
-      </c>
-      <c r="G33" s="21">
+      <c r="F33" s="12">
+        <v>0</v>
+      </c>
+      <c r="G33" s="19">
         <f t="shared" ref="G33:G39" si="5">F33*C33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="17">
+      <c r="B34" s="15">
         <v>3</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="10">
         <v>120</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="9">
         <v>3</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="10">
         <f t="shared" si="4"/>
         <v>360</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="12">
         <v>2</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="19">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="17">
+      <c r="B35" s="15">
         <v>5</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="10">
         <v>300</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="9">
         <v>1</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="10">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="12">
         <v>1</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="19">
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="17">
+      <c r="B36" s="15">
         <v>8</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="10">
         <v>720</v>
       </c>
-      <c r="D36" s="11">
-        <v>0</v>
-      </c>
-      <c r="E36" s="12">
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="12">
         <v>2</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="19">
         <f t="shared" si="5"/>
         <v>1440</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="17">
+      <c r="B37" s="15">
         <v>13</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="10">
         <v>1440</v>
       </c>
-      <c r="D37" s="11">
-        <v>0</v>
-      </c>
-      <c r="E37" s="12">
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F37" s="14">
-        <v>0</v>
-      </c>
-      <c r="G37" s="21">
+      <c r="F37" s="12">
+        <v>0</v>
+      </c>
+      <c r="G37" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="17">
+      <c r="B38" s="15">
         <v>21</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="10">
         <f>2.5*24*60</f>
         <v>3600</v>
       </c>
-      <c r="D38" s="11">
-        <v>0</v>
-      </c>
-      <c r="E38" s="12">
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F38" s="14">
-        <v>0</v>
-      </c>
-      <c r="G38" s="21">
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="17">
+      <c r="B39" s="15">
         <v>40</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="10">
         <f>7*24*60</f>
         <v>10080</v>
       </c>
-      <c r="D39" s="11">
-        <v>0</v>
-      </c>
-      <c r="E39" s="12">
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F39" s="14">
-        <v>0</v>
-      </c>
-      <c r="G39" s="22">
+      <c r="F39" s="12">
+        <v>0</v>
+      </c>
+      <c r="G39" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="4"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="7" t="s">
+      <c r="B40" s="3"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="4">
         <f>SUM(E32:E39)/60</f>
         <v>11.75</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G40" s="17">
         <f>SUM(G32:G39)/60</f>
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="16">
+      <c r="B46" s="14">
         <v>1</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="8">
         <v>15</v>
       </c>
-      <c r="D46" s="9">
-        <v>0</v>
-      </c>
-      <c r="E46" s="10">
+      <c r="D46" s="7">
+        <v>0</v>
+      </c>
+      <c r="E46" s="8">
         <f>D46*C46</f>
         <v>0</v>
       </c>
-      <c r="F46" s="13">
-        <v>0</v>
-      </c>
-      <c r="G46" s="20">
+      <c r="F46" s="11">
+        <v>0</v>
+      </c>
+      <c r="G46" s="18">
         <f>F46*C46</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="17">
+      <c r="B47" s="15">
         <v>2</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="10">
         <v>45</v>
       </c>
-      <c r="D47" s="11">
+      <c r="D47" s="9">
         <v>1</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="10">
         <f t="shared" ref="E47:E53" si="6">D47*C47</f>
         <v>45</v>
       </c>
-      <c r="F47" s="14">
-        <v>0</v>
-      </c>
-      <c r="G47" s="21">
+      <c r="F47" s="12">
+        <v>0</v>
+      </c>
+      <c r="G47" s="19">
         <f t="shared" ref="G47:G53" si="7">F47*C47</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="17">
+      <c r="B48" s="15">
         <v>3</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="10">
         <v>120</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="9">
         <v>4</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="10">
         <f t="shared" si="6"/>
         <v>480</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="12">
         <v>2</v>
       </c>
-      <c r="G48" s="21">
+      <c r="G48" s="19">
         <f t="shared" si="7"/>
         <v>240</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="17">
+      <c r="B49" s="15">
         <v>5</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C49" s="10">
         <v>300</v>
       </c>
-      <c r="D49" s="11">
-        <v>0</v>
-      </c>
-      <c r="E49" s="12">
+      <c r="D49" s="9">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="12">
         <v>3</v>
       </c>
-      <c r="G49" s="21">
+      <c r="G49" s="19">
         <f t="shared" si="7"/>
         <v>900</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="17">
+      <c r="B50" s="15">
         <v>8</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50" s="10">
         <v>720</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="9">
         <v>1</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="10">
         <f t="shared" si="6"/>
         <v>720</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="12">
         <v>1</v>
       </c>
-      <c r="G50" s="21">
+      <c r="G50" s="19">
         <f t="shared" si="7"/>
         <v>720</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="17">
+      <c r="B51" s="15">
         <v>13</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51" s="10">
         <v>1440</v>
       </c>
-      <c r="D51" s="11">
-        <v>0</v>
-      </c>
-      <c r="E51" s="12">
+      <c r="D51" s="9">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F51" s="14">
-        <v>0</v>
-      </c>
-      <c r="G51" s="21">
+      <c r="F51" s="12">
+        <v>0</v>
+      </c>
+      <c r="G51" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="17">
+      <c r="B52" s="15">
         <v>21</v>
       </c>
-      <c r="C52" s="12">
+      <c r="C52" s="10">
         <f>2.5*24*60</f>
         <v>3600</v>
       </c>
-      <c r="D52" s="11">
-        <v>0</v>
-      </c>
-      <c r="E52" s="12">
+      <c r="D52" s="9">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F52" s="14">
-        <v>0</v>
-      </c>
-      <c r="G52" s="21">
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="17">
+      <c r="B53" s="15">
         <v>40</v>
       </c>
-      <c r="C53" s="12">
+      <c r="C53" s="10">
         <f>7*24*60</f>
         <v>10080</v>
       </c>
-      <c r="D53" s="11">
-        <v>0</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="D53" s="9">
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F53" s="14">
-        <v>0</v>
-      </c>
-      <c r="G53" s="22">
+      <c r="F53" s="12">
+        <v>0</v>
+      </c>
+      <c r="G53" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="4"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="7" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="4">
         <f>SUM(E46:E53)/60</f>
         <v>20.75</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G54" s="19">
+      <c r="G54" s="17">
         <f>SUM(G46:G53)/60</f>
         <v>31</v>
       </c>
     </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+    </row>
+    <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="14">
+        <v>1</v>
+      </c>
+      <c r="C60" s="8">
+        <v>15</v>
+      </c>
+      <c r="D60" s="7">
+        <v>1</v>
+      </c>
+      <c r="E60" s="8">
+        <f>D60*C60</f>
+        <v>15</v>
+      </c>
+      <c r="F60" s="11">
+        <v>1</v>
+      </c>
+      <c r="G60" s="18">
+        <f>F60*C60</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="15">
+        <v>2</v>
+      </c>
+      <c r="C61" s="10">
+        <v>45</v>
+      </c>
+      <c r="D61" s="9">
+        <v>5</v>
+      </c>
+      <c r="E61" s="10">
+        <f t="shared" ref="E61:E67" si="8">D61*C61</f>
+        <v>225</v>
+      </c>
+      <c r="F61" s="12">
+        <v>3</v>
+      </c>
+      <c r="G61" s="19">
+        <f t="shared" ref="G61:G67" si="9">F61*C61</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="15">
+        <v>3</v>
+      </c>
+      <c r="C62" s="10">
+        <v>120</v>
+      </c>
+      <c r="D62" s="9">
+        <v>2</v>
+      </c>
+      <c r="E62" s="10">
+        <f t="shared" si="8"/>
+        <v>240</v>
+      </c>
+      <c r="F62" s="12">
+        <v>4</v>
+      </c>
+      <c r="G62" s="19">
+        <f t="shared" si="9"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="15">
+        <v>5</v>
+      </c>
+      <c r="C63" s="10">
+        <v>300</v>
+      </c>
+      <c r="D63" s="9">
+        <v>1</v>
+      </c>
+      <c r="E63" s="10">
+        <f t="shared" si="8"/>
+        <v>300</v>
+      </c>
+      <c r="F63" s="12">
+        <v>1</v>
+      </c>
+      <c r="G63" s="19">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="15">
+        <v>8</v>
+      </c>
+      <c r="C64" s="10">
+        <v>720</v>
+      </c>
+      <c r="D64" s="9">
+        <v>2</v>
+      </c>
+      <c r="E64" s="10">
+        <f t="shared" si="8"/>
+        <v>1440</v>
+      </c>
+      <c r="F64" s="12">
+        <v>2</v>
+      </c>
+      <c r="G64" s="19">
+        <f t="shared" si="9"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="15">
+        <v>13</v>
+      </c>
+      <c r="C65" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0</v>
+      </c>
+      <c r="E65" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0</v>
+      </c>
+      <c r="G65" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="15">
+        <v>21</v>
+      </c>
+      <c r="C66" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0</v>
+      </c>
+      <c r="E66" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0</v>
+      </c>
+      <c r="G66" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="15">
+        <v>40</v>
+      </c>
+      <c r="C67" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0</v>
+      </c>
+      <c r="E67" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="3"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="4">
+        <f>SUM(E60:E67)/60</f>
+        <v>37</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" s="17">
+        <f>SUM(G60:G67)/60</f>
+        <v>39.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B15:G16"/>
     <mergeCell ref="B29:G30"/>
     <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 5 #50
</commit_message>
<xml_diff>
--- a/docs/md/anexos/Registro-tiempo.xlsx
+++ b/docs/md/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -339,149 +345,471 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="98">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1159,8 +1487,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="69" headerRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="97" headerRowBorderDxfId="96">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B3:G12">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1180,9 +1552,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1202,16 +1574,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B31:G40">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
     <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
@@ -1224,31 +1589,24 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="25"/>
+    <tableColumn id="2" name="Min." dataDxfId="22" totalsRowDxfId="23"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="20" totalsRowDxfId="21"/>
+    <tableColumn id="4" name="Total" dataDxfId="18" totalsRowDxfId="19"/>
+    <tableColumn id="5" name="Real" dataDxfId="16" totalsRowDxfId="17"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
     <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
@@ -1524,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G68"/>
+  <dimension ref="B1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,8 +3069,478 @@
         <v>39.5</v>
       </c>
     </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+    </row>
+    <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+    </row>
+    <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="14">
+        <v>1</v>
+      </c>
+      <c r="C74" s="8">
+        <v>15</v>
+      </c>
+      <c r="D74" s="7">
+        <v>1</v>
+      </c>
+      <c r="E74" s="8">
+        <f>D74*C74</f>
+        <v>15</v>
+      </c>
+      <c r="F74" s="11">
+        <v>1</v>
+      </c>
+      <c r="G74" s="18">
+        <f>F74*C74</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="15">
+        <v>2</v>
+      </c>
+      <c r="C75" s="10">
+        <v>45</v>
+      </c>
+      <c r="D75" s="9">
+        <v>1</v>
+      </c>
+      <c r="E75" s="10">
+        <f t="shared" ref="E75:E81" si="10">D75*C75</f>
+        <v>45</v>
+      </c>
+      <c r="F75" s="12">
+        <v>1</v>
+      </c>
+      <c r="G75" s="19">
+        <f t="shared" ref="G75:G81" si="11">F75*C75</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="15">
+        <v>3</v>
+      </c>
+      <c r="C76" s="10">
+        <v>120</v>
+      </c>
+      <c r="D76" s="9">
+        <v>2</v>
+      </c>
+      <c r="E76" s="10">
+        <f t="shared" si="10"/>
+        <v>240</v>
+      </c>
+      <c r="F76" s="12">
+        <v>2</v>
+      </c>
+      <c r="G76" s="19">
+        <f t="shared" si="11"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="15">
+        <v>5</v>
+      </c>
+      <c r="C77" s="10">
+        <v>300</v>
+      </c>
+      <c r="D77" s="9">
+        <v>2</v>
+      </c>
+      <c r="E77" s="10">
+        <f t="shared" si="10"/>
+        <v>600</v>
+      </c>
+      <c r="F77" s="12">
+        <v>1</v>
+      </c>
+      <c r="G77" s="19">
+        <f t="shared" si="11"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="15">
+        <v>8</v>
+      </c>
+      <c r="C78" s="10">
+        <v>720</v>
+      </c>
+      <c r="D78" s="9">
+        <v>1</v>
+      </c>
+      <c r="E78" s="10">
+        <f t="shared" si="10"/>
+        <v>720</v>
+      </c>
+      <c r="F78" s="12">
+        <v>2</v>
+      </c>
+      <c r="G78" s="19">
+        <f t="shared" si="11"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="15">
+        <v>13</v>
+      </c>
+      <c r="C79" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="12">
+        <v>0</v>
+      </c>
+      <c r="G79" s="19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="15">
+        <v>21</v>
+      </c>
+      <c r="C80" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D80" s="9">
+        <v>0</v>
+      </c>
+      <c r="E80" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="12">
+        <v>0</v>
+      </c>
+      <c r="G80" s="19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="15">
+        <v>40</v>
+      </c>
+      <c r="C81" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0</v>
+      </c>
+      <c r="E81" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="12">
+        <v>0</v>
+      </c>
+      <c r="G81" s="20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="3"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" s="4">
+        <f>SUM(E74:E81)/60</f>
+        <v>27</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82" s="17">
+        <f>SUM(G74:G81)/60</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+    </row>
+    <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="14">
+        <v>1</v>
+      </c>
+      <c r="C88" s="8">
+        <v>15</v>
+      </c>
+      <c r="D88" s="7">
+        <v>1</v>
+      </c>
+      <c r="E88" s="8">
+        <f>D88*C88</f>
+        <v>15</v>
+      </c>
+      <c r="F88" s="11">
+        <v>1</v>
+      </c>
+      <c r="G88" s="18">
+        <f>F88*C88</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="15">
+        <v>2</v>
+      </c>
+      <c r="C89" s="10">
+        <v>45</v>
+      </c>
+      <c r="D89" s="9">
+        <v>2</v>
+      </c>
+      <c r="E89" s="10">
+        <f t="shared" ref="E89:E95" si="12">D89*C89</f>
+        <v>90</v>
+      </c>
+      <c r="F89" s="12">
+        <v>1</v>
+      </c>
+      <c r="G89" s="19">
+        <f t="shared" ref="G89:G95" si="13">F89*C89</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="15">
+        <v>3</v>
+      </c>
+      <c r="C90" s="10">
+        <v>120</v>
+      </c>
+      <c r="D90" s="9">
+        <v>1</v>
+      </c>
+      <c r="E90" s="10">
+        <f t="shared" si="12"/>
+        <v>120</v>
+      </c>
+      <c r="F90" s="12">
+        <v>2</v>
+      </c>
+      <c r="G90" s="19">
+        <f t="shared" si="13"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="15">
+        <v>5</v>
+      </c>
+      <c r="C91" s="10">
+        <v>300</v>
+      </c>
+      <c r="D91" s="9">
+        <v>1</v>
+      </c>
+      <c r="E91" s="10">
+        <f t="shared" si="12"/>
+        <v>300</v>
+      </c>
+      <c r="F91" s="12">
+        <v>0</v>
+      </c>
+      <c r="G91" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="15">
+        <v>8</v>
+      </c>
+      <c r="C92" s="10">
+        <v>720</v>
+      </c>
+      <c r="D92" s="9">
+        <v>1</v>
+      </c>
+      <c r="E92" s="10">
+        <f t="shared" si="12"/>
+        <v>720</v>
+      </c>
+      <c r="F92" s="12">
+        <v>1</v>
+      </c>
+      <c r="G92" s="19">
+        <f t="shared" si="13"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="15">
+        <v>13</v>
+      </c>
+      <c r="C93" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D93" s="9">
+        <v>0</v>
+      </c>
+      <c r="E93" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F93" s="12">
+        <v>1</v>
+      </c>
+      <c r="G93" s="19">
+        <f t="shared" si="13"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="15">
+        <v>21</v>
+      </c>
+      <c r="C94" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D94" s="9">
+        <v>0</v>
+      </c>
+      <c r="E94" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F94" s="12">
+        <v>0</v>
+      </c>
+      <c r="G94" s="19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="15">
+        <v>40</v>
+      </c>
+      <c r="C95" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D95" s="9">
+        <v>0</v>
+      </c>
+      <c r="E95" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F95" s="12">
+        <v>0</v>
+      </c>
+      <c r="G95" s="20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="3"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96" s="4">
+        <f>SUM(E88:E95)/60</f>
+        <v>20.75</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96" s="17">
+        <f>SUM(G88:G95)/60</f>
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B71:G72"/>
+    <mergeCell ref="B85:G86"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B15:G16"/>
     <mergeCell ref="B29:G30"/>
@@ -2721,12 +3549,14 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 8 #65
</commit_message>
<xml_diff>
--- a/docs/md/anexos/Registro-tiempo.xlsx
+++ b/docs/md/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="16">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -70,12 +70,15 @@
   <si>
     <t>Sprint 7</t>
   </si>
+  <si>
+    <t>Sprint 8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +121,14 @@
       <u/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -347,162 +358,324 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="112">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="126">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1663,8 +1836,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="111" headerRowBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="125" headerRowBorderDxfId="124">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="4" name="Total" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="5" name="Real" dataDxfId="115" totalsRowDxfId="114"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1684,9 +1879,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1706,9 +1901,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1728,16 +1923,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
@@ -1750,9 +1938,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
     <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
@@ -1765,9 +1953,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
     <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
@@ -1780,9 +1968,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
     <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
@@ -1795,9 +1983,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
     <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
@@ -2073,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G110"/>
+  <dimension ref="B1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,22 +2275,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -2325,22 +2513,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -2559,22 +2747,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -2793,22 +2981,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -3027,22 +3215,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -3261,22 +3449,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -3495,22 +3683,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="22"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -3729,22 +3917,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="21"/>
-      <c r="F99" s="21"/>
-      <c r="G99" s="21"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="22"/>
-      <c r="C100" s="22"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -3913,7 +4101,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F108" s="23">
+      <c r="F108" s="21">
         <v>0</v>
       </c>
       <c r="G108" s="19">
@@ -3962,8 +4150,246 @@
         <v>23</v>
       </c>
     </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="22"/>
+    </row>
+    <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
+    </row>
+    <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="14">
+        <v>1</v>
+      </c>
+      <c r="C116" s="8">
+        <v>15</v>
+      </c>
+      <c r="D116" s="7">
+        <v>0</v>
+      </c>
+      <c r="E116" s="8">
+        <f>D116*C116</f>
+        <v>0</v>
+      </c>
+      <c r="F116" s="11">
+        <v>0</v>
+      </c>
+      <c r="G116" s="18">
+        <f>F116*C116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="15">
+        <v>2</v>
+      </c>
+      <c r="C117" s="10">
+        <v>45</v>
+      </c>
+      <c r="D117" s="9">
+        <v>0</v>
+      </c>
+      <c r="E117" s="10">
+        <f t="shared" ref="E117:E123" si="16">D117*C117</f>
+        <v>0</v>
+      </c>
+      <c r="F117" s="12">
+        <v>0</v>
+      </c>
+      <c r="G117" s="19">
+        <f t="shared" ref="G117:G123" si="17">F117*C117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="15">
+        <v>3</v>
+      </c>
+      <c r="C118" s="10">
+        <v>120</v>
+      </c>
+      <c r="D118" s="9">
+        <v>0</v>
+      </c>
+      <c r="E118" s="10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="12">
+        <v>0</v>
+      </c>
+      <c r="G118" s="19">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="15">
+        <v>5</v>
+      </c>
+      <c r="C119" s="10">
+        <v>300</v>
+      </c>
+      <c r="D119" s="9">
+        <v>2</v>
+      </c>
+      <c r="E119" s="10">
+        <f t="shared" si="16"/>
+        <v>600</v>
+      </c>
+      <c r="F119" s="12">
+        <v>1</v>
+      </c>
+      <c r="G119" s="19">
+        <f t="shared" si="17"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="15">
+        <v>8</v>
+      </c>
+      <c r="C120" s="10">
+        <v>720</v>
+      </c>
+      <c r="D120" s="9">
+        <v>3</v>
+      </c>
+      <c r="E120" s="10">
+        <f t="shared" si="16"/>
+        <v>2160</v>
+      </c>
+      <c r="F120" s="12">
+        <v>4</v>
+      </c>
+      <c r="G120" s="19">
+        <f t="shared" si="17"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="15">
+        <v>13</v>
+      </c>
+      <c r="C121" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D121" s="9">
+        <v>0</v>
+      </c>
+      <c r="E121" s="10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F121" s="12">
+        <v>0</v>
+      </c>
+      <c r="G121" s="19">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="15">
+        <v>21</v>
+      </c>
+      <c r="C122" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D122" s="9">
+        <v>0</v>
+      </c>
+      <c r="E122" s="10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F122" s="21">
+        <v>0</v>
+      </c>
+      <c r="G122" s="19">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="15">
+        <v>40</v>
+      </c>
+      <c r="C123" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D123" s="9">
+        <v>0</v>
+      </c>
+      <c r="E123" s="10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F123" s="12">
+        <v>0</v>
+      </c>
+      <c r="G123" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="3"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E124" s="4">
+        <f>SUM(E116:E123)/60</f>
+        <v>46</v>
+      </c>
+      <c r="F124" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G124" s="17">
+        <f>SUM(G116:G123)/60</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F128" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B113:G114"/>
     <mergeCell ref="B99:G100"/>
     <mergeCell ref="B71:G72"/>
     <mergeCell ref="B85:G86"/>
@@ -3975,7 +4401,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3984,6 +4410,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document Sprint 9, Tecnicas y herramientas and minor improvements #72 #73
</commit_message>
<xml_diff>
--- a/docs/md/anexos/Registro-tiempo.xlsx
+++ b/docs/md/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="17">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -73,12 +73,15 @@
   <si>
     <t>Sprint 8</t>
   </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,14 +124,6 @@
       <u/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -367,154 +362,314 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="140">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1836,8 +1991,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="125" headerRowBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="139" headerRowBorderDxfId="138">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
+    <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="4" name="Total" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="5" name="Real" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="126"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1857,9 +2049,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1879,9 +2071,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1901,16 +2093,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
     <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
@@ -1923,9 +2108,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
@@ -1938,9 +2123,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
     <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
@@ -1953,9 +2138,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
     <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
@@ -1968,9 +2153,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
     <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
@@ -1978,21 +2163,6 @@
     <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2261,10 +2431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G128"/>
+  <dimension ref="B1:G138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,11 +4554,243 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F128" s="24"/>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" s="22"/>
+      <c r="D127" s="22"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="22"/>
+      <c r="G127" s="22"/>
+    </row>
+    <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="23"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="23"/>
+    </row>
+    <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="14">
+        <v>1</v>
+      </c>
+      <c r="C130" s="8">
+        <v>15</v>
+      </c>
+      <c r="D130" s="7">
+        <v>1</v>
+      </c>
+      <c r="E130" s="8">
+        <f>D130*C130</f>
+        <v>15</v>
+      </c>
+      <c r="F130" s="11">
+        <v>1</v>
+      </c>
+      <c r="G130" s="18">
+        <f>F130*C130</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="15">
+        <v>2</v>
+      </c>
+      <c r="C131" s="10">
+        <v>45</v>
+      </c>
+      <c r="D131" s="9">
+        <v>1</v>
+      </c>
+      <c r="E131" s="10">
+        <f t="shared" ref="E131:E137" si="18">D131*C131</f>
+        <v>45</v>
+      </c>
+      <c r="F131" s="12">
+        <v>0</v>
+      </c>
+      <c r="G131" s="19">
+        <f t="shared" ref="G131:G137" si="19">F131*C131</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="15">
+        <v>3</v>
+      </c>
+      <c r="C132" s="10">
+        <v>120</v>
+      </c>
+      <c r="D132" s="9">
+        <v>0</v>
+      </c>
+      <c r="E132" s="10">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F132" s="12">
+        <v>1</v>
+      </c>
+      <c r="G132" s="19">
+        <f t="shared" si="19"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="15">
+        <v>5</v>
+      </c>
+      <c r="C133" s="10">
+        <v>300</v>
+      </c>
+      <c r="D133" s="9">
+        <v>2</v>
+      </c>
+      <c r="E133" s="10">
+        <f t="shared" si="18"/>
+        <v>600</v>
+      </c>
+      <c r="F133" s="12">
+        <v>2</v>
+      </c>
+      <c r="G133" s="19">
+        <f t="shared" si="19"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="15">
+        <v>8</v>
+      </c>
+      <c r="C134" s="10">
+        <v>720</v>
+      </c>
+      <c r="D134" s="9">
+        <v>1</v>
+      </c>
+      <c r="E134" s="10">
+        <f t="shared" si="18"/>
+        <v>720</v>
+      </c>
+      <c r="F134" s="12">
+        <v>1</v>
+      </c>
+      <c r="G134" s="19">
+        <f t="shared" si="19"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="15">
+        <v>13</v>
+      </c>
+      <c r="C135" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D135" s="9">
+        <v>0</v>
+      </c>
+      <c r="E135" s="10">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F135" s="12">
+        <v>0</v>
+      </c>
+      <c r="G135" s="19">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B136" s="15">
+        <v>21</v>
+      </c>
+      <c r="C136" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D136" s="9">
+        <v>0</v>
+      </c>
+      <c r="E136" s="10">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F136" s="21">
+        <v>0</v>
+      </c>
+      <c r="G136" s="19">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="15">
+        <v>40</v>
+      </c>
+      <c r="C137" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D137" s="9">
+        <v>0</v>
+      </c>
+      <c r="E137" s="10">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F137" s="12">
+        <v>0</v>
+      </c>
+      <c r="G137" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="3"/>
+      <c r="C138" s="16"/>
+      <c r="D138" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E138" s="4">
+        <f>SUM(E130:E137)/60</f>
+        <v>23</v>
+      </c>
+      <c r="F138" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G138" s="17">
+        <f>SUM(G130:G137)/60</f>
+        <v>24.25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B127:G128"/>
     <mergeCell ref="B113:G114"/>
     <mergeCell ref="B99:G100"/>
     <mergeCell ref="B71:G72"/>
@@ -4401,7 +4803,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4411,6 +4813,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document sprint 10 #81
</commit_message>
<xml_diff>
--- a/docs/md/anexos/Registro-tiempo.xlsx
+++ b/docs/md/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -76,6 +76,9 @@
   <si>
     <t>Sprint 9</t>
   </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
 </sst>
 </file>
 
@@ -120,10 +123,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <u/>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -353,162 +355,323 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="140">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+  <dxfs count="154">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1991,8 +2154,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="139" headerRowBorderDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="153" headerRowBorderDxfId="152">
   <autoFilter ref="B17:G26">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
+    <tableColumn id="2" name="Min." dataDxfId="149" totalsRowDxfId="148"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="147" totalsRowDxfId="146"/>
+    <tableColumn id="4" name="Total" dataDxfId="145" totalsRowDxfId="144"/>
+    <tableColumn id="5" name="Real" dataDxfId="143" totalsRowDxfId="142"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="141" totalsRowDxfId="140"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2012,24 +2227,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B3:G12">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2049,9 +2249,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B31:G40">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B45:G54">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2071,16 +2271,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B45:G54">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
     <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
@@ -2093,9 +2286,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
     <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
@@ -2108,9 +2301,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
@@ -2123,9 +2316,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B101:G110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
     <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
@@ -2138,9 +2331,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B115:G124"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
     <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
@@ -2148,21 +2341,6 @@
     <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
     <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B115:G124"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -2431,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G138"/>
+  <dimension ref="B1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="J119" sqref="J119"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,22 +2623,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -2683,22 +2861,22 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -2917,22 +3095,22 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
@@ -3151,22 +3329,22 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -3385,22 +3563,22 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="23"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
@@ -3619,22 +3797,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="22"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
     </row>
     <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
@@ -3853,22 +4031,22 @@
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
     </row>
     <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="23"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
     </row>
     <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
@@ -4087,22 +4265,22 @@
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="23"/>
-      <c r="C100" s="23"/>
-      <c r="D100" s="23"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -4271,7 +4449,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F108" s="21">
+      <c r="F108" s="12">
         <v>0</v>
       </c>
       <c r="G108" s="19">
@@ -4321,22 +4499,22 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
-      <c r="G113" s="22"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="21"/>
     </row>
     <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="23"/>
-      <c r="C114" s="23"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="23"/>
+      <c r="B114" s="22"/>
+      <c r="C114" s="22"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
+      <c r="G114" s="22"/>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
@@ -4505,7 +4683,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F122" s="21">
+      <c r="F122" s="12">
         <v>0</v>
       </c>
       <c r="G122" s="19">
@@ -4555,22 +4733,22 @@
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="22"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="22"/>
-      <c r="G127" s="22"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="23"/>
-      <c r="C128" s="23"/>
-      <c r="D128" s="23"/>
-      <c r="E128" s="23"/>
-      <c r="F128" s="23"/>
-      <c r="G128" s="23"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="22"/>
+      <c r="G128" s="22"/>
     </row>
     <row r="129" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -4739,7 +4917,7 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="F136" s="21">
+      <c r="F136" s="12">
         <v>0</v>
       </c>
       <c r="G136" s="19">
@@ -4788,22 +4966,257 @@
         <v>24.25</v>
       </c>
     </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141" s="21"/>
+      <c r="D141" s="21"/>
+      <c r="E141" s="21"/>
+      <c r="F141" s="21"/>
+      <c r="G141" s="21"/>
+    </row>
+    <row r="142" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="22"/>
+      <c r="C142" s="22"/>
+      <c r="D142" s="22"/>
+      <c r="E142" s="22"/>
+      <c r="F142" s="22"/>
+      <c r="G142" s="22"/>
+    </row>
+    <row r="143" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G143" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B144" s="14">
+        <v>1</v>
+      </c>
+      <c r="C144" s="8">
+        <v>15</v>
+      </c>
+      <c r="D144" s="7">
+        <v>1</v>
+      </c>
+      <c r="E144" s="8">
+        <f>D144*C144</f>
+        <v>15</v>
+      </c>
+      <c r="F144" s="11">
+        <v>1</v>
+      </c>
+      <c r="G144" s="18">
+        <f>F144*C144</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B145" s="15">
+        <v>2</v>
+      </c>
+      <c r="C145" s="10">
+        <v>45</v>
+      </c>
+      <c r="D145" s="9">
+        <v>2</v>
+      </c>
+      <c r="E145" s="10">
+        <f t="shared" ref="E145:E151" si="20">D145*C145</f>
+        <v>90</v>
+      </c>
+      <c r="F145" s="12">
+        <v>0</v>
+      </c>
+      <c r="G145" s="19">
+        <f t="shared" ref="G145:G151" si="21">F145*C145</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B146" s="15">
+        <v>3</v>
+      </c>
+      <c r="C146" s="10">
+        <v>120</v>
+      </c>
+      <c r="D146" s="9">
+        <v>0</v>
+      </c>
+      <c r="E146" s="10">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F146" s="12">
+        <v>1</v>
+      </c>
+      <c r="G146" s="19">
+        <f t="shared" si="21"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B147" s="15">
+        <v>5</v>
+      </c>
+      <c r="C147" s="10">
+        <v>300</v>
+      </c>
+      <c r="D147" s="9">
+        <v>4</v>
+      </c>
+      <c r="E147" s="10">
+        <f t="shared" si="20"/>
+        <v>1200</v>
+      </c>
+      <c r="F147" s="12">
+        <v>5</v>
+      </c>
+      <c r="G147" s="19">
+        <f t="shared" si="21"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B148" s="15">
+        <v>8</v>
+      </c>
+      <c r="C148" s="10">
+        <v>720</v>
+      </c>
+      <c r="D148" s="9">
+        <v>1</v>
+      </c>
+      <c r="E148" s="10">
+        <f t="shared" si="20"/>
+        <v>720</v>
+      </c>
+      <c r="F148" s="12">
+        <v>1</v>
+      </c>
+      <c r="G148" s="19">
+        <f t="shared" si="21"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B149" s="15">
+        <v>13</v>
+      </c>
+      <c r="C149" s="10">
+        <v>1440</v>
+      </c>
+      <c r="D149" s="9">
+        <v>0</v>
+      </c>
+      <c r="E149" s="10">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F149" s="12">
+        <v>0</v>
+      </c>
+      <c r="G149" s="19">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B150" s="15">
+        <v>21</v>
+      </c>
+      <c r="C150" s="10">
+        <f>2.5*24*60</f>
+        <v>3600</v>
+      </c>
+      <c r="D150" s="9">
+        <v>0</v>
+      </c>
+      <c r="E150" s="10">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F150" s="12">
+        <v>0</v>
+      </c>
+      <c r="G150" s="19">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="15">
+        <v>40</v>
+      </c>
+      <c r="C151" s="10">
+        <f>7*24*60</f>
+        <v>10080</v>
+      </c>
+      <c r="D151" s="9">
+        <v>0</v>
+      </c>
+      <c r="E151" s="10">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F151" s="12">
+        <v>0</v>
+      </c>
+      <c r="G151" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="3"/>
+      <c r="C152" s="16"/>
+      <c r="D152" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E152" s="4">
+        <f>SUM(E144:E151)/60</f>
+        <v>33.75</v>
+      </c>
+      <c r="F152" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G152" s="23">
+        <f>SUM(G144:G151)/60</f>
+        <v>39.25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B141:G142"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
     <mergeCell ref="B127:G128"/>
     <mergeCell ref="B113:G114"/>
     <mergeCell ref="B99:G100"/>
     <mergeCell ref="B71:G72"/>
     <mergeCell ref="B85:G86"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="B57:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="10">
+  <tableParts count="11">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4814,6 +5227,7 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>